<commit_message>
Use colors to highlight mandatory fields in metadata
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F27630-12B8-4921-B4AE-686264D9EA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE7A5C3-DF18-44D8-9BAE-978F572B69C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -1043,7 +1043,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1062,6 +1062,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1075,7 +1087,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1085,11 +1097,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1107,6 +1132,14 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1126,7 +1159,7 @@
   <autoFilter ref="A1:B11" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{197420D8-A12C-4324-87A4-2BEAC3F2FAF6}" name="name_raw"/>
-    <tableColumn id="2" xr3:uid="{9CEB246F-9418-43C1-93E4-E01091B6A441}" name="name_new"/>
+    <tableColumn id="2" xr3:uid="{9CEB246F-9418-43C1-93E4-E01091B6A441}" name="name_new" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1138,7 +1171,7 @@
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{E993CBC8-A1B1-4E4C-8906-7171AD5EB8DA}" name="event_id"/>
     <tableColumn id="3" xr3:uid="{2C30F1DE-E33C-48DF-B5EA-F221EFC19502}" name="event_id_pattern"/>
-    <tableColumn id="5" xr3:uid="{B8744317-3956-4F39-A2A1-F571FB40341F}" name="is_regular_visit" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{B8744317-3956-4F39-A2A1-F571FB40341F}" name="is_regular_visit" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{BC267C30-A507-48B0-8B2A-ABC6EB4A6D66}" name="event_label_custom"/>
     <tableColumn id="1" xr3:uid="{76BD4AA6-095B-46B4-AD1F-74CB4B63B7A1}" name="event_name_custom"/>
     <tableColumn id="4" xr3:uid="{BC23E39F-CE6F-4D20-AF70-E0E9D2B9A5E8}" name="is_baseline_event"/>
@@ -1152,7 +1185,7 @@
   <autoFilter ref="A1:E51" xr:uid="{3DC8495A-80F1-47D0-B099-A4444169C84F}"/>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{32D2D5DB-90F1-452A-A407-9958F05DFC29}" name="var"/>
-    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{DDF6B9DA-22E8-4772-BC2A-2E79D78BA24F}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{78F87B1B-3FB5-4BDA-8075-9F2908D15BE4}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{D15D9292-219E-4D48-9449-CA4B7E84D719}" name="item_group"/>
@@ -1169,13 +1202,13 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="12" xr3:uid="{3F460AD3-FCC0-44D5-BBE7-96068C605604}" name="var"/>
-    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{CFD88543-6276-40D6-9487-D6A7385190F4}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{E0E61225-3F35-4968-A99C-26C9994CEE9F}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{9E97B4D1-3E86-442C-9084-2E44749A5442}" name="item_group"/>
     <tableColumn id="4" xr3:uid="{17ACC2A8-A45A-49FD-AC66-881A4CCD7E07}" name="unit"/>
-    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1188,7 +1221,7 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{5604E1C1-7286-42A9-9446-BD07C4022CD9}" name="var"/>
-    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{EE82524D-5440-46D2-ABCD-5FFB7844C279}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{29DD0374-4740-492E-9A7C-90F52163213A}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{F6C07853-FBDF-4C62-8817-4C93F651B74A}" name="item_group"/>
@@ -1211,7 +1244,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B16" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:B16" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
     <sortCondition ref="B1:B15"/>
@@ -1521,103 +1554,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>254</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>255</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>256</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>257</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>258</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>259</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>260</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>261</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>262</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>263</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>243</v>
       </c>
     </row>
@@ -1631,25 +1667,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47507AE3-65CF-4352-8C5A-A70367C9C41D}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>265</v>
       </c>
@@ -1669,7 +1708,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>287</v>
       </c>
@@ -1683,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>296</v>
       </c>
@@ -1700,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>297</v>
       </c>
@@ -1717,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>298</v>
       </c>
@@ -1734,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>299</v>
       </c>
@@ -1751,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>300</v>
       </c>
@@ -1768,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>301</v>
       </c>
@@ -1785,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>288</v>
       </c>
@@ -1802,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>290</v>
       </c>
@@ -1816,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>292</v>
       </c>
@@ -1841,43 +1880,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2EDD7A-5ED3-4521-BBD0-E5535A4AFBF0}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1891,11 +1933,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>217</v>
       </c>
       <c r="D3" t="s">
@@ -1905,7 +1947,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1919,11 +1961,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>91</v>
       </c>
       <c r="D5" t="s">
@@ -1933,11 +1975,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D6" t="s">
@@ -1947,11 +1989,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>92</v>
       </c>
       <c r="D7" t="s">
@@ -1961,11 +2003,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>215</v>
       </c>
       <c r="D8" t="s">
@@ -1975,11 +2017,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>88</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>216</v>
       </c>
       <c r="D9" t="s">
@@ -1989,7 +2031,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2003,7 +2045,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -2017,7 +2059,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>211</v>
       </c>
@@ -2031,11 +2073,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>218</v>
       </c>
       <c r="D13" t="s">
@@ -2045,7 +2087,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>220</v>
       </c>
@@ -2059,11 +2101,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>98</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>103</v>
       </c>
       <c r="D15" t="s">
@@ -2073,7 +2115,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -2087,7 +2129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>212</v>
       </c>
@@ -2101,7 +2143,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -2115,7 +2157,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -2129,7 +2171,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -2143,7 +2185,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -2157,7 +2199,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -2171,7 +2213,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>198</v>
       </c>
@@ -2185,7 +2227,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>213</v>
       </c>
@@ -2199,7 +2241,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -2213,7 +2255,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -2227,7 +2269,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>151</v>
       </c>
@@ -2241,7 +2283,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>153</v>
       </c>
@@ -2255,7 +2297,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>155</v>
       </c>
@@ -2269,7 +2311,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>157</v>
       </c>
@@ -2283,7 +2325,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>158</v>
       </c>
@@ -2297,7 +2339,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>161</v>
       </c>
@@ -2311,7 +2353,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>163</v>
       </c>
@@ -2325,7 +2367,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>165</v>
       </c>
@@ -2339,7 +2381,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -2353,7 +2395,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>146</v>
       </c>
@@ -2367,7 +2409,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>167</v>
       </c>
@@ -2381,11 +2423,11 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>169</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D38" t="s">
@@ -2395,7 +2437,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>170</v>
       </c>
@@ -2409,7 +2451,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>178</v>
       </c>
@@ -2423,7 +2465,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2437,7 +2479,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>181</v>
       </c>
@@ -2451,7 +2493,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>172</v>
       </c>
@@ -2465,7 +2507,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>173</v>
       </c>
@@ -2479,7 +2521,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>184</v>
       </c>
@@ -2493,11 +2535,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>187</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="6" t="s">
         <v>225</v>
       </c>
       <c r="D46" t="s">
@@ -2507,7 +2549,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>188</v>
       </c>
@@ -2521,7 +2563,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>190</v>
       </c>
@@ -2535,7 +2577,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>192</v>
       </c>
@@ -2549,7 +2591,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>194</v>
       </c>
@@ -2563,7 +2605,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>195</v>
       </c>
@@ -2588,42 +2630,45 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB3F453-AEAC-4610-ADFE-EC9F8781793B}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>204</v>
       </c>
       <c r="D1" t="s">
         <v>205</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>206</v>
       </c>
       <c r="F1" t="s">
@@ -2636,7 +2681,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2662,7 +2707,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2688,7 +2733,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2714,7 +2759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2740,7 +2785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2766,7 +2811,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2783,7 +2828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2809,7 +2854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2835,7 +2880,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2852,7 +2897,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2869,7 +2914,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2886,7 +2931,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2903,7 +2948,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2920,7 +2965,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2937,7 +2982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2954,7 +2999,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2971,7 +3016,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2988,7 +3033,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3005,7 +3050,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3022,7 +3067,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -3039,7 +3084,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -3056,7 +3101,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3073,7 +3118,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -3090,7 +3135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3107,7 +3152,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -3124,7 +3169,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3141,7 +3186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -3158,7 +3203,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>208</v>
       </c>
@@ -3172,7 +3217,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>209</v>
       </c>
@@ -3197,99 +3242,102 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D649F3-3138-4439-A355-CAB4EEAE2B78}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="A8:E8"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>111</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -3303,21 +3351,21 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3331,7 +3379,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -3345,7 +3393,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3359,7 +3407,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -3373,7 +3421,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -3387,21 +3435,21 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -3415,35 +3463,35 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>122</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -3457,7 +3505,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -3471,7 +3519,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -3485,7 +3533,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3499,7 +3547,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -3524,36 +3572,39 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB008CF7-ADB1-4FBF-A44E-B95C9F0C41E8}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3567,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -3581,7 +3632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -3595,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3609,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3623,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -3648,27 +3699,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FFF7FA-E437-4B11-81D1-BE338C7C5391}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -3676,7 +3730,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>251</v>
       </c>
@@ -3684,7 +3738,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -3692,7 +3746,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -3700,7 +3754,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>274</v>
       </c>
@@ -3708,7 +3762,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -3716,7 +3770,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>249</v>
       </c>
@@ -3724,7 +3778,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -3732,7 +3786,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>241</v>
       </c>
@@ -3740,7 +3794,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>253</v>
       </c>
@@ -3748,7 +3802,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>246</v>
       </c>
@@ -3756,7 +3810,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>233</v>
       </c>
@@ -3764,7 +3818,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>236</v>
       </c>
@@ -3772,7 +3826,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>247</v>
       </c>
@@ -3780,7 +3834,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>271</v>
       </c>
@@ -3798,21 +3852,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>277</v>
       </c>
@@ -3829,7 +3886,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>278</v>
       </c>

</xml_diff>

<commit_message>
Color more metadata columns orange as appropriate
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CCDF2D-083A-463D-97C5-415F7C4C8B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8557AB-0083-478A-BE85-DE690A776ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -2636,8 +2636,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,7 +2666,7 @@
       <c r="C1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>205</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -3248,7 +3248,7 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3579,7 +3579,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update metadata so that merge_with handles all pre-exisitng 'other' columns
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A40C8F-9D5D-435B-8360-C25C0BBE8E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A85FA8-8B79-42D0-B3BB-0C583C4C2C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="318">
   <si>
     <t>continuous</t>
   </si>
@@ -565,9 +565,6 @@
     <t>CM_CMTRT</t>
   </si>
   <si>
-    <t>CM Trade Name</t>
-  </si>
-  <si>
     <t>CM_MHREL</t>
   </si>
   <si>
@@ -589,9 +586,6 @@
     <t>CM_CMDOSU_OTH</t>
   </si>
   <si>
-    <t>CM Unit Other</t>
-  </si>
-  <si>
     <t>CM_CMDOSFRQ</t>
   </si>
   <si>
@@ -601,9 +595,6 @@
     <t>CM_CMDOSFRQ_OTH</t>
   </si>
   <si>
-    <t>CM Frequency Other</t>
-  </si>
-  <si>
     <t>CM_CMROUTE</t>
   </si>
   <si>
@@ -613,9 +604,6 @@
     <t>CM Route</t>
   </si>
   <si>
-    <t>CM Route Other</t>
-  </si>
-  <si>
     <t>CM_CMSTDAT</t>
   </si>
   <si>
@@ -730,9 +718,6 @@
     <t>CM_CMINGRD</t>
   </si>
   <si>
-    <t>CM Active Ingredient</t>
-  </si>
-  <si>
     <t>event_label</t>
   </si>
   <si>
@@ -862,9 +847,6 @@
     <t>AE Treatment related</t>
   </si>
   <si>
-    <t>AE Other action</t>
-  </si>
-  <si>
     <t>MH Name</t>
   </si>
   <si>
@@ -1040,6 +1022,12 @@
   </si>
   <si>
     <t>\U1F48A T\U2093</t>
+  </si>
+  <si>
+    <t>merge_with</t>
+  </si>
+  <si>
+    <t>CM Name</t>
   </si>
 </sst>
 </file>
@@ -1149,14 +1137,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98DE20DA-3AF1-43CC-B81F-9C209EFD7E17}" name="Table264" displayName="Table264" ref="A1:E51" totalsRowShown="0">
-  <autoFilter ref="A1:E51" xr:uid="{3DC8495A-80F1-47D0-B099-A4444169C84F}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98DE20DA-3AF1-43CC-B81F-9C209EFD7E17}" name="Table264" displayName="Table264" ref="A1:F46" totalsRowShown="0">
+  <autoFilter ref="A1:F46" xr:uid="{3DC8495A-80F1-47D0-B099-A4444169C84F}"/>
+  <tableColumns count="6">
     <tableColumn id="12" xr3:uid="{32D2D5DB-90F1-452A-A407-9958F05DFC29}" name="var"/>
     <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{DDF6B9DA-22E8-4772-BC2A-2E79D78BA24F}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{78F87B1B-3FB5-4BDA-8075-9F2908D15BE4}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{D15D9292-219E-4D48-9449-CA4B7E84D719}" name="item_group"/>
+    <tableColumn id="1" xr3:uid="{91CCE224-6ABA-4020-B0FC-2FB8B66C8177}" name="merge_with"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1534,71 +1523,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B4" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B7" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1606,18 +1595,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B10" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -1648,10 +1637,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1659,10 +1648,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1673,7 +1662,7 @@
         <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1684,7 +1673,7 @@
         <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1695,7 +1684,7 @@
         <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1706,7 +1695,7 @@
         <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,7 +1706,7 @@
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1728,7 +1717,7 @@
         <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1739,7 +1728,7 @@
         <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1750,7 +1739,7 @@
         <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1761,7 +1750,7 @@
         <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1772,7 +1761,7 @@
         <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1783,7 +1772,7 @@
         <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1794,7 +1783,7 @@
         <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,7 +1794,7 @@
         <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1816,7 +1805,7 @@
         <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,7 +1816,7 @@
         <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,7 +1827,7 @@
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,7 +1838,7 @@
         <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1860,7 +1849,7 @@
         <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1874,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2EDD7A-5ED3-4521-BBD0-E5535A4AFBF0}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,13 +1876,13 @@
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1901,21 +1890,24 @@
         <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="F1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
@@ -1924,12 +1916,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D3" t="s">
         <v>40</v>
@@ -1938,7 +1930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1952,7 +1944,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -1966,7 +1958,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -1980,7 +1972,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -1994,12 +1986,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -2008,12 +2000,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -2022,12 +2014,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -2036,12 +2028,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -2049,13 +2041,16 @@
       <c r="E11" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D12" t="s">
         <v>40</v>
@@ -2064,12 +2059,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>253</v>
       </c>
       <c r="C13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>
@@ -2078,12 +2073,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>122</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -2092,12 +2087,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s">
         <v>40</v>
@@ -2106,12 +2101,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
         <v>40</v>
@@ -2120,12 +2115,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>250</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>259</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
         <v>40</v>
@@ -2134,12 +2129,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="D18" t="s">
         <v>40</v>
@@ -2148,12 +2143,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D19" t="s">
         <v>40</v>
@@ -2162,219 +2157,231 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>267</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
         <v>40</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>213</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>317</v>
       </c>
       <c r="D21" t="s">
         <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="F21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>162</v>
+        <v>246</v>
       </c>
       <c r="C22" t="s">
+        <v>247</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>235</v>
+      </c>
+      <c r="F24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
+        <v>235</v>
+      </c>
+      <c r="F25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>235</v>
+      </c>
+      <c r="F26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" t="s">
+        <v>181</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>163</v>
       </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>217</v>
-      </c>
-      <c r="C23" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>251</v>
-      </c>
-      <c r="C24" t="s">
-        <v>252</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>166</v>
-      </c>
-      <c r="C25" t="s">
-        <v>167</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" t="s">
-        <v>169</v>
-      </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>170</v>
-      </c>
-      <c r="C27" t="s">
-        <v>171</v>
-      </c>
-      <c r="D27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>172</v>
-      </c>
-      <c r="C28" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>174</v>
-      </c>
-      <c r="C29" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>176</v>
-      </c>
       <c r="C30" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D31" t="s">
         <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D32" t="s">
         <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
-        <v>183</v>
+        <v>258</v>
       </c>
       <c r="D33" t="s">
         <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D34" t="s">
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="C35" t="s">
         <v>194</v>
@@ -2383,231 +2390,161 @@
         <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="C36" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D36" t="s">
         <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="C37" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="D37" t="s">
         <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C38" t="s">
-        <v>264</v>
+        <v>192</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
       </c>
       <c r="E38" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D39" t="s">
         <v>40</v>
       </c>
       <c r="E39" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D40" t="s">
         <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C41" t="s">
+        <v>257</v>
+      </c>
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" t="s">
         <v>201</v>
-      </c>
-      <c r="D41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C42" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D42" t="s">
         <v>40</v>
       </c>
       <c r="E42" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C43" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="D43" t="s">
         <v>40</v>
       </c>
       <c r="E43" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="C44" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D44" t="s">
         <v>40</v>
       </c>
       <c r="E44" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C45" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D45" t="s">
         <v>40</v>
       </c>
       <c r="E45" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C46" t="s">
-        <v>263</v>
+        <v>212</v>
       </c>
       <c r="D46" t="s">
         <v>40</v>
       </c>
       <c r="E46" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>207</v>
-      </c>
-      <c r="C47" t="s">
-        <v>208</v>
-      </c>
-      <c r="D47" t="s">
-        <v>40</v>
-      </c>
-      <c r="E47" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>209</v>
-      </c>
-      <c r="C48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E48" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>211</v>
-      </c>
-      <c r="C49" t="s">
-        <v>212</v>
-      </c>
-      <c r="D49" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>213</v>
-      </c>
-      <c r="C50" t="s">
-        <v>215</v>
-      </c>
-      <c r="D50" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>214</v>
-      </c>
-      <c r="C51" t="s">
-        <v>216</v>
-      </c>
-      <c r="D51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E51" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2624,7 +2561,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,13 +2588,13 @@
         <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F1" t="s">
         <v>32</v>
@@ -3193,7 +3130,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C29" t="s">
         <v>93</v>
@@ -3207,10 +3144,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C30" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -3233,7 +3170,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="A8:E8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3257,13 +3194,13 @@
         <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3574,16 +3511,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C1" t="s">
         <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3695,119 +3632,119 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" t="s">
         <v>269</v>
-      </c>
-      <c r="B1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B11" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B12" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B14" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B15" t="s">
         <v>95</v>
@@ -3815,10 +3752,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B16" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3833,7 +3770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3847,33 +3784,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" t="s">
         <v>314</v>
-      </c>
-      <c r="E1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add study_name to the metadata template
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4193D83A-7660-46D9-98D6-58B74AD4FFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA74CE-7336-4FD7-86F2-6EDC3AEEA899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="311">
   <si>
     <t>continuous</t>
   </si>
@@ -1004,6 +1004,9 @@
   </si>
   <si>
     <t>CM Name</t>
+  </si>
+  <si>
+    <t>study_name</t>
   </si>
 </sst>
 </file>
@@ -1100,11 +1103,12 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1114,11 +1118,7 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1128,11 +1128,33 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1150,12 +1172,11 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1164,24 +1185,6 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1197,21 +1200,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:B11" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:B11" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{197420D8-A12C-4324-87A4-2BEAC3F2FAF6}" name="name_raw"/>
-    <tableColumn id="2" xr3:uid="{9CEB246F-9418-43C1-93E4-E01091B6A441}" name="name_new" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{9CEB246F-9418-43C1-93E4-E01091B6A441}" name="name_new" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FAB0EA66-5868-4938-9FA9-F93E72C101B3}" name="Table913" displayName="Table913" ref="A1:F11" totalsRowShown="0" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FAB0EA66-5868-4938-9FA9-F93E72C101B3}" name="Table913" displayName="Table913" ref="A1:F11" totalsRowShown="0" headerRowBorderDxfId="12">
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{E993CBC8-A1B1-4E4C-8906-7171AD5EB8DA}" name="event_id"/>
     <tableColumn id="3" xr3:uid="{2C30F1DE-E33C-48DF-B5EA-F221EFC19502}" name="event_id_pattern"/>
-    <tableColumn id="5" xr3:uid="{B8744317-3956-4F39-A2A1-F571FB40341F}" name="is_regular_visit" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{B8744317-3956-4F39-A2A1-F571FB40341F}" name="is_regular_visit" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{BC267C30-A507-48B0-8B2A-ABC6EB4A6D66}" name="event_label_custom"/>
     <tableColumn id="1" xr3:uid="{76BD4AA6-095B-46B4-AD1F-74CB4B63B7A1}" name="event_name_custom"/>
     <tableColumn id="4" xr3:uid="{BC23E39F-CE6F-4D20-AF70-E0E9D2B9A5E8}" name="is_baseline_event"/>
@@ -1221,10 +1224,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CDCCBD4-1725-47F3-8EB1-67F674961D0F}" name="Table2642" displayName="Table2642" ref="A1:F46" totalsRowShown="0" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CDCCBD4-1725-47F3-8EB1-67F674961D0F}" name="Table2642" displayName="Table2642" ref="A1:F46" totalsRowShown="0" headerRowBorderDxfId="10">
   <tableColumns count="6">
     <tableColumn id="12" xr3:uid="{06CD6130-2807-4D21-89F8-47575A27637D}" name="var"/>
-    <tableColumn id="11" xr3:uid="{C40E9486-CC28-43B0-8094-303D73716F92}" name="suffix" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{C40E9486-CC28-43B0-8094-303D73716F92}" name="suffix" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{B5EA8893-F567-4544-BAC4-B107EC3D4EA2}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{EB3138FA-83B5-4EF2-BE9F-78559AC53839}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{E2FFC47A-4930-4565-9670-F6729DE8D6A9}" name="item_group"/>
@@ -1235,32 +1238,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE818089-4D49-40C3-B6E9-CD667DF15A15}" name="Table2654" displayName="Table2654" ref="A1:H30" totalsRowShown="0" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE818089-4D49-40C3-B6E9-CD667DF15A15}" name="Table2654" displayName="Table2654" ref="A1:H30" totalsRowShown="0" headerRowBorderDxfId="8">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D22">
     <sortCondition ref="D1:D22"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="12" xr3:uid="{836D48CB-BA99-47A1-960C-7887CD4F176A}" name="var"/>
-    <tableColumn id="11" xr3:uid="{766A85FE-E078-435B-BD2C-3E104D0FE1D2}" name="suffix" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{766A85FE-E078-435B-BD2C-3E104D0FE1D2}" name="suffix" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{AE994462-4BA4-4F11-AC6A-FC883A074DE0}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{3E31C7A4-0ACC-4E98-A1E1-92BE6B5ED083}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{B1091BB7-3720-43DE-8A90-9AD515F1CAB3}" name="item_group"/>
     <tableColumn id="4" xr3:uid="{F1F11124-9A68-4A46-933C-36E897EEC80F}" name="unit"/>
-    <tableColumn id="5" xr3:uid="{A57ED687-02A8-4F73-A504-A0AAD705069C}" name="lower_limit" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{BE802246-F4D1-4845-8110-212C64BC1602}" name="upper_limit" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{A57ED687-02A8-4F73-A504-A0AAD705069C}" name="lower_limit" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BE802246-F4D1-4845-8110-212C64BC1602}" name="upper_limit" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A1F288F2-B4AB-420E-BAFE-FEF3F7C9D929}" name="Table267" displayName="Table267" ref="A1:E21" totalsRowShown="0" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A1F288F2-B4AB-420E-BAFE-FEF3F7C9D929}" name="Table267" displayName="Table267" ref="A1:E21" totalsRowShown="0" headerRowBorderDxfId="4">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
     <sortCondition ref="D1:D21"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{5604E1C1-7286-42A9-9446-BD07C4022CD9}" name="var"/>
-    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{EE82524D-5440-46D2-ABCD-5FFB7844C279}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{29DD0374-4740-492E-9A7C-90F52163213A}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{F6C07853-FBDF-4C62-8817-4C93F651B74A}" name="item_group"/>
@@ -1270,7 +1273,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7AED27C5-CB47-4830-8F47-BB9354073F14}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0" headerRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7AED27C5-CB47-4830-8F47-BB9354073F14}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0" headerRowBorderDxfId="2">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D16F68B8-5C50-48F1-9AAD-869306EF0109}" name="item_group"/>
     <tableColumn id="3" xr3:uid="{C44DD745-DA94-43D6-993D-55FB6C28A7E6}" name="item_scale"/>
@@ -1282,7 +1285,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B16" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B16" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
     <sortCondition ref="B1:B15"/>
   </sortState>
@@ -1600,13 +1603,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>263</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>248</v>
       </c>
@@ -1622,7 +1625,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>250</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>251</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>252</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>253</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>254</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>256</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>257</v>
       </c>
@@ -1713,19 +1716,19 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>259</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>281</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>290</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>291</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>292</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>295</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>282</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>284</v>
       </c>
@@ -1892,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>286</v>
       </c>
@@ -1926,20 +1929,20 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -2043,7 +2046,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2057,7 +2060,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -2102,7 +2105,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -2116,7 +2119,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>207</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -2200,7 +2203,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -2228,7 +2231,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>194</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>208</v>
       </c>
@@ -2259,7 +2262,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -2273,7 +2276,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>151</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>154</v>
       </c>
@@ -2324,7 +2327,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>157</v>
       </c>
@@ -2338,7 +2341,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>159</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>161</v>
       </c>
@@ -2366,7 +2369,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -2380,7 +2383,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -2450,7 +2453,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>176</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>168</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>180</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>183</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>184</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -2576,7 +2579,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>190</v>
       </c>
@@ -2590,7 +2593,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>191</v>
       </c>
@@ -2624,23 +2627,23 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2692,7 +2695,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2718,7 +2721,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2744,7 +2747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2770,7 +2773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2796,7 +2799,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2839,7 +2842,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2865,7 +2868,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2916,7 +2919,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2933,7 +2936,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2950,7 +2953,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2967,7 +2970,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -3001,7 +3004,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3035,7 +3038,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3052,7 +3055,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -3086,7 +3089,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3103,7 +3106,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -3120,7 +3123,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -3154,7 +3157,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3171,7 +3174,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -3188,7 +3191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>203</v>
       </c>
@@ -3202,7 +3205,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>204</v>
       </c>
@@ -3236,20 +3239,20 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -3280,7 +3283,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -3336,7 +3339,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -3350,7 +3353,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3364,7 +3367,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -3378,7 +3381,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3392,7 +3395,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -3420,7 +3423,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -3434,7 +3437,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -3476,7 +3479,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -3490,7 +3493,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -3504,7 +3507,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -3532,7 +3535,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -3566,16 +3569,16 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>201</v>
       </c>
@@ -3589,7 +3592,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3603,7 +3606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -3617,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -3631,7 +3634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3645,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3659,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -3693,13 +3696,13 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>225</v>
       </c>
@@ -3707,7 +3710,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>238</v>
       </c>
@@ -3715,7 +3718,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>245</v>
       </c>
@@ -3723,7 +3726,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>236</v>
       </c>
@@ -3731,7 +3734,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>236</v>
       </c>
@@ -3739,7 +3742,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -3747,7 +3750,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>228</v>
       </c>
@@ -3755,7 +3758,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>243</v>
       </c>
@@ -3763,7 +3766,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>233</v>
       </c>
@@ -3771,7 +3774,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -3779,7 +3782,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>247</v>
       </c>
@@ -3787,7 +3790,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>240</v>
       </c>
@@ -3795,7 +3798,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>227</v>
       </c>
@@ -3803,7 +3806,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>230</v>
       </c>
@@ -3811,7 +3814,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>241</v>
       </c>
@@ -3819,7 +3822,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>265</v>
       </c>
@@ -3840,21 +3843,20 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>271</v>
       </c>
@@ -3870,8 +3872,11 @@
       <c r="E1" s="3" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>272</v>
       </c>

</xml_diff>

<commit_message>
Adjust metadata so that the SAE table order resembles more the old state
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA74CE-7336-4FD7-86F2-6EDC3AEEA899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B845613-96D4-4CBB-B081-6D24774C4180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -1599,7 +1599,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1925,9 +1925,7 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2121,10 +2119,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C13" t="s">
-        <v>214</v>
+        <v>98</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -2135,10 +2133,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
@@ -2149,10 +2147,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>216</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -2163,10 +2161,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Remove outcome column from metadata instead since it is not populated in clinsight metadata
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B845613-96D4-4CBB-B081-6D24774C4180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13EFE0C-A5AF-4431-A76E-0DF1CA1E1BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="309">
   <si>
     <t>continuous</t>
   </si>
@@ -374,12 +374,6 @@
   </si>
   <si>
     <t>AE_AESER_ENDAT</t>
-  </si>
-  <si>
-    <t>AE_AESER_AEOUT</t>
-  </si>
-  <si>
-    <t>SAE outcome</t>
   </si>
   <si>
     <t>SAE End date</t>
@@ -1224,7 +1218,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CDCCBD4-1725-47F3-8EB1-67F674961D0F}" name="Table2642" displayName="Table2642" ref="A1:F46" totalsRowShown="0" headerRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CDCCBD4-1725-47F3-8EB1-67F674961D0F}" name="Table2642" displayName="Table2642" ref="A1:F45" totalsRowShown="0" headerRowBorderDxfId="10">
   <tableColumns count="6">
     <tableColumn id="12" xr3:uid="{06CD6130-2807-4D21-89F8-47575A27637D}" name="var"/>
     <tableColumn id="11" xr3:uid="{C40E9486-CC28-43B0-8094-303D73716F92}" name="suffix" dataDxfId="9"/>
@@ -1611,71 +1605,71 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
@@ -1683,18 +1677,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -1730,33 +1724,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>280</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1764,16 +1758,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1781,16 +1775,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1798,16 +1792,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1815,16 +1809,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1832,16 +1826,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1849,16 +1843,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1866,16 +1860,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1883,13 +1877,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1897,13 +1891,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1923,7 +1917,7 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1948,16 +1942,16 @@
         <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>201</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,7 +1959,7 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
@@ -1979,7 +1973,7 @@
         <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
@@ -2049,7 +2043,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -2063,7 +2057,7 @@
         <v>88</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D9" t="s">
         <v>39</v>
@@ -2077,7 +2071,7 @@
         <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
@@ -2091,7 +2085,7 @@
         <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D11" t="s">
         <v>39</v>
@@ -2100,7 +2094,7 @@
         <v>84</v>
       </c>
       <c r="F11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2108,7 +2102,7 @@
         <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>
@@ -2122,7 +2116,7 @@
         <v>98</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -2136,7 +2130,7 @@
         <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
@@ -2147,10 +2141,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -2161,10 +2155,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -2175,10 +2169,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -2189,10 +2183,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D18" t="s">
         <v>39</v>
@@ -2203,61 +2197,61 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>223</v>
+        <v>140</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" t="s">
+        <v>307</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>195</v>
+      </c>
+      <c r="F20" t="s">
         <v>141</v>
-      </c>
-      <c r="C20" t="s">
-        <v>142</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>309</v>
+        <v>207</v>
       </c>
       <c r="D21" t="s">
         <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>197</v>
-      </c>
-      <c r="F21" t="s">
-        <v>143</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>209</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,38 +2265,41 @@
         <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>197</v>
+        <v>195</v>
+      </c>
+      <c r="F23" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D24" t="s">
         <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F25" t="s">
         <v>153</v>
@@ -2310,7 +2307,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C26" t="s">
         <v>156</v>
@@ -2319,10 +2316,7 @@
         <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>197</v>
-      </c>
-      <c r="F26" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2336,7 +2330,7 @@
         <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2350,49 +2344,49 @@
         <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D30" t="s">
         <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2400,41 +2394,41 @@
         <v>163</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
+        <v>218</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
       </c>
       <c r="E32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" t="s">
         <v>165</v>
       </c>
-      <c r="C33" t="s">
-        <v>220</v>
-      </c>
       <c r="D33" t="s">
         <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D34" t="s">
         <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,97 +2436,97 @@
         <v>174</v>
       </c>
       <c r="C35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D35" t="s">
         <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
         <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
       </c>
       <c r="E37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D38" t="s">
         <v>39</v>
       </c>
       <c r="E38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C39" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D39" t="s">
         <v>39</v>
       </c>
       <c r="E39" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" t="s">
+        <v>217</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" t="s">
         <v>180</v>
-      </c>
-      <c r="C40" t="s">
-        <v>181</v>
-      </c>
-      <c r="D40" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" t="s">
         <v>183</v>
       </c>
-      <c r="C41" t="s">
-        <v>219</v>
-      </c>
       <c r="D41" t="s">
         <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2546,7 +2540,7 @@
         <v>39</v>
       </c>
       <c r="E42" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2560,7 +2554,7 @@
         <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,41 +2562,27 @@
         <v>188</v>
       </c>
       <c r="C44" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D44" t="s">
         <v>39</v>
       </c>
       <c r="E44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D45" t="s">
         <v>39</v>
       </c>
       <c r="E45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>191</v>
-      </c>
-      <c r="C46" t="s">
-        <v>193</v>
-      </c>
-      <c r="D46" t="s">
-        <v>39</v>
-      </c>
-      <c r="E46" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2649,13 +2629,13 @@
         <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>201</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>31</v>
@@ -3191,7 +3171,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C29" t="s">
         <v>74</v>
@@ -3205,10 +3185,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D30" t="s">
         <v>39</v>
@@ -3258,41 +3238,41 @@
         <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3306,35 +3286,35 @@
         <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3348,7 +3328,7 @@
         <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3362,189 +3342,189 @@
         <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" t="s">
         <v>116</v>
       </c>
-      <c r="C9" t="s">
-        <v>118</v>
-      </c>
       <c r="D9" t="s">
         <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
         <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
         <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
         <v>136</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
         <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3578,16 +3558,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>79</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3702,119 +3682,119 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B15" t="s">
         <v>76</v>
@@ -3822,10 +3802,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3856,36 +3836,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>273</v>
-      </c>
       <c r="C1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" t="s">
         <v>275</v>
-      </c>
-      <c r="D2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" t="s">
-        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update study status label in tables
(cherry picked from commit fca5a75d418da1dc3b4dd046c0cce88de9c322da)
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13EFE0C-A5AF-4431-A76E-0DF1CA1E1BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D673B1-D5C7-4862-839A-3F61506A6136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="6" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="311">
   <si>
     <t>continuous</t>
   </si>
@@ -1001,6 +1001,12 @@
   </si>
   <si>
     <t>study_name</t>
+  </si>
+  <si>
+    <t>Study Status</t>
+  </si>
+  <si>
+    <t>study_status</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1285,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B16" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B17" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
     <sortCondition ref="B1:B15"/>
   </sortState>
@@ -1597,13 +1603,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>261</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>247</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>248</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>249</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>250</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>251</v>
       </c>
@@ -1659,7 +1665,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>252</v>
       </c>
@@ -1667,7 +1673,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>253</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>254</v>
       </c>
@@ -1683,7 +1689,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>255</v>
       </c>
@@ -1710,19 +1716,19 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>257</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -1773,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -1807,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>292</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>293</v>
       </c>
@@ -1858,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>282</v>
       </c>
@@ -1889,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>284</v>
       </c>
@@ -1919,22 +1925,22 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1968,7 +1974,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1982,7 +1988,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -2024,7 +2030,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -2038,7 +2044,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2052,7 +2058,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -2066,7 +2072,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2080,7 +2086,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -2097,7 +2103,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2139,7 +2145,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>205</v>
       </c>
@@ -2153,7 +2159,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>213</v>
       </c>
@@ -2167,7 +2173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>139</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>206</v>
       </c>
@@ -2240,7 +2246,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -2254,7 +2260,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -2271,7 +2277,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -2288,7 +2294,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>152</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>155</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>157</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>159</v>
       </c>
@@ -2347,7 +2353,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -2375,7 +2381,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>161</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2417,7 +2423,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -2431,7 +2437,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>175</v>
       </c>
@@ -2459,7 +2465,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2473,7 +2479,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>167</v>
       </c>
@@ -2487,7 +2493,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>181</v>
       </c>
@@ -2515,7 +2521,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>182</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>184</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -2557,7 +2563,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -2571,7 +2577,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -2605,23 +2611,23 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2725,7 +2731,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2777,7 +2783,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2794,7 +2800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2820,7 +2826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2897,7 +2903,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2931,7 +2937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2999,7 +3005,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3016,7 +3022,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -3050,7 +3056,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3084,7 +3090,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3118,7 +3124,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -3135,7 +3141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3152,7 +3158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>201</v>
       </c>
@@ -3183,7 +3189,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>202</v>
       </c>
@@ -3217,20 +3223,20 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -3247,7 +3253,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -3261,7 +3267,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -3275,7 +3281,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -3289,7 +3295,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -3317,7 +3323,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3345,7 +3351,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -3373,7 +3379,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -3387,7 +3393,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -3401,7 +3407,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -3415,7 +3421,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -3429,7 +3435,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -3443,7 +3449,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -3457,7 +3463,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>115</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -3485,7 +3491,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -3499,7 +3505,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -3513,7 +3519,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -3547,16 +3553,16 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>199</v>
       </c>
@@ -3570,7 +3576,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -3598,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -3612,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3626,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3640,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -3668,19 +3674,17 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>223</v>
       </c>
@@ -3688,7 +3692,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -3696,7 +3700,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>243</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>234</v>
       </c>
@@ -3712,7 +3716,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>234</v>
       </c>
@@ -3720,7 +3724,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>266</v>
       </c>
@@ -3728,7 +3732,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>226</v>
       </c>
@@ -3736,7 +3740,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>241</v>
       </c>
@@ -3744,7 +3748,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>231</v>
       </c>
@@ -3752,7 +3756,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>233</v>
       </c>
@@ -3760,7 +3764,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>245</v>
       </c>
@@ -3768,7 +3772,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>238</v>
       </c>
@@ -3776,7 +3780,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>225</v>
       </c>
@@ -3784,7 +3788,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>228</v>
       </c>
@@ -3792,7 +3796,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>239</v>
       </c>
@@ -3800,12 +3804,20 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>263</v>
       </c>
       <c r="B16" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3825,16 +3837,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>269</v>
       </c>
@@ -3854,7 +3866,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>270</v>
       </c>

</xml_diff>

<commit_message>
Rename study status table label in metadata to subject status
</commit_message>
<xml_diff>
--- a/inst/metadata.xlsx
+++ b/inst/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99_data_science\clinsight\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D673B1-D5C7-4862-839A-3F61506A6136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DA7F2B-2EC7-46BF-ABC6-229D82EB79C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="6" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -1003,10 +1003,10 @@
     <t>study_name</t>
   </si>
   <si>
-    <t>Study Status</t>
-  </si>
-  <si>
-    <t>study_status</t>
+    <t>subject_status</t>
+  </si>
+  <si>
+    <t>Subject Status</t>
   </si>
 </sst>
 </file>
@@ -1603,13 +1603,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>261</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>247</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>248</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>249</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>250</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>251</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>252</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>253</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>254</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>255</v>
       </c>
@@ -1716,19 +1716,19 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>257</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>279</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>292</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>293</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>282</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>284</v>
       </c>
@@ -1927,20 +1927,20 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>205</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>213</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>139</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>206</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>152</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>155</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>157</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>159</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>161</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>175</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>167</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>181</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>182</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>184</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -2611,23 +2611,23 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>201</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>202</v>
       </c>
@@ -3223,20 +3223,20 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>115</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -3553,16 +3553,16 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>199</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -3676,15 +3676,17 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>223</v>
       </c>
@@ -3692,7 +3694,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -3700,7 +3702,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>243</v>
       </c>
@@ -3708,7 +3710,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>234</v>
       </c>
@@ -3716,7 +3718,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>234</v>
       </c>
@@ -3724,7 +3726,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>266</v>
       </c>
@@ -3732,7 +3734,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>226</v>
       </c>
@@ -3740,7 +3742,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>241</v>
       </c>
@@ -3748,7 +3750,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>231</v>
       </c>
@@ -3756,7 +3758,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>233</v>
       </c>
@@ -3764,7 +3766,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>245</v>
       </c>
@@ -3772,7 +3774,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>238</v>
       </c>
@@ -3780,7 +3782,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>225</v>
       </c>
@@ -3788,7 +3790,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>228</v>
       </c>
@@ -3796,7 +3798,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>239</v>
       </c>
@@ -3804,7 +3806,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>263</v>
       </c>
@@ -3812,12 +3814,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>310</v>
+      </c>
+      <c r="B17" t="s">
         <v>309</v>
-      </c>
-      <c r="B17" t="s">
-        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3837,16 +3839,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>269</v>
       </c>
@@ -3866,7 +3868,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>270</v>
       </c>

</xml_diff>